<commit_message>
Uppdatering av html, kartläggninsgfrågor och försdjupning för föräldratsöd
</commit_message>
<xml_diff>
--- a/docs/Kartläggning_fldr.xlsx
+++ b/docs/Kartläggning_fldr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarala/DIDsteg2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDA262F-EEFD-E040-8339-51F9EBD21F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6240A2-BB22-3F42-9EA1-19E190FACED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="1040" windowWidth="27840" windowHeight="16020" xr2:uid="{7BC09E43-1041-714B-B107-1A982B11F32C}"/>
+    <workbookView xWindow="620" yWindow="2500" windowWidth="27840" windowHeight="16020" xr2:uid="{7BC09E43-1041-714B-B107-1A982B11F32C}"/>
   </bookViews>
   <sheets>
     <sheet name="Kartläggande frågor" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
   <si>
     <t>Datum</t>
   </si>
@@ -89,36 +89,12 @@
     <t>Annat:</t>
   </si>
   <si>
-    <t>Specifika modeller, metoder, verktyg eller bedömningsinstrument används under samtalen.</t>
-  </si>
-  <si>
-    <t>Tidiga samordnade insatser (TSI)</t>
-  </si>
-  <si>
-    <t>Det finns en kommunövergripande plan för arbetet med tidiga samordnade insatser.</t>
-  </si>
-  <si>
-    <t>Det finns en samverkansöverenskommelse mellan skola, hälso- och sjukvård, socialtjänst, fritidsverksamhet och polis.</t>
-  </si>
-  <si>
     <t>Vårdnadshavare och barn och unga involveras i arbetet.</t>
   </si>
   <si>
-    <t>Det finns ett tvärsektoriellt team.</t>
-  </si>
-  <si>
-    <t>Det erbjuds kunskapshöjande insatser om tidiga samordnade insatser.</t>
-  </si>
-  <si>
-    <t>Det finns kommunövergripande rutiner för samverkan med andra föräldraskapsstödjande aktörer såsom socialtjänst och hälso- och sjukvård.</t>
-  </si>
-  <si>
     <t>Utökat hembesöksprogram</t>
   </si>
   <si>
-    <t>Det finns mål/strategier för arbetet med utökat hembesöksprogram.</t>
-  </si>
-  <si>
     <t>Det finns långsiktig finansiering för arbetet  med utökat hembesöksprogram.</t>
   </si>
   <si>
@@ -134,27 +110,15 @@
     <t>Det finns en eller flera familjecentraler i kommunen.</t>
   </si>
   <si>
-    <t>Mål/strategier för arbetDet finns mål/strategier för arbetet med familjecentraler.et med familjecentraler</t>
-  </si>
-  <si>
     <t>Det finns långsiktig finansiering av familjecentraler.</t>
   </si>
   <si>
-    <t>Uppföljning görs av vilka som besöker familjecentralen.</t>
-  </si>
-  <si>
-    <t>Uppföljning görs av familjecentralens resultat för barn och föräldrar</t>
-  </si>
-  <si>
     <t>Öppen förskola</t>
   </si>
   <si>
     <t>Det finns en eller flera öppna förskolor i kommunen.</t>
   </si>
   <si>
-    <t>Det finns mål/strategier för arbetet med öppen förskola.</t>
-  </si>
-  <si>
     <t>Det görs kontinuerlig uppföljning av vilka som besöker den öppna förskolan.</t>
   </si>
   <si>
@@ -167,21 +131,12 @@
     <t>Det finns en kommunövergripande plan för förskolans och skolans samverkan med föräldrar</t>
   </si>
   <si>
-    <t>Kommnen erbjuder personalen kunskapshöjande insatser om föräldraskapsstöd och föräldrasamverkan</t>
-  </si>
-  <si>
-    <t>Det finns kommunövergripande rutiner för samverkan med andra föräldraskapsstödjande aktörer såsom socialtjänst och hälso- och sjukvård</t>
-  </si>
-  <si>
     <t>Respektive förskola/skola har en gemensam strategi för att möjliggöra för hem och vårdnadshavare att bli delaktiga i frågor som rör elevens skolgång.</t>
   </si>
   <si>
     <t>Respektive förskola/skola har gemensamma förhållningssätt i kontakter med vårdnadshavare och hemmen</t>
   </si>
   <si>
-    <t>Det erbjuds kunskapshöjande insatser till förskola/skola om föräldraskapsstöd och föräldrasamverkan.</t>
-  </si>
-  <si>
     <t>Föräldrar i kommunen erbjuds föräldragrupp via MHV respektive BHV.</t>
   </si>
   <si>
@@ -191,19 +146,7 @@
     <t>Det finns långsiktig finansiering för arbetet med föräldragrupper.</t>
   </si>
   <si>
-    <t>Uppföljning görs av vilka som deltar i föräldragrupper på MHV respektive BHV.</t>
-  </si>
-  <si>
-    <t>Uppföljning görs av vilka resultat som grupperna får för barn och föräldrar.</t>
-  </si>
-  <si>
-    <t>Det finns mål/strategier för arbetet med föräldragrupper.</t>
-  </si>
-  <si>
     <t>Triple P</t>
-  </si>
-  <si>
-    <t>Det finns mål/strategier för arbetet med universella föräldraskapsstödsprogram.</t>
   </si>
   <si>
     <r>
@@ -274,19 +217,7 @@
     <t>Föräldraföreläsningar</t>
   </si>
   <si>
-    <t>Det finns det mål/strategier för arbetet med föräldraföreläsningar.</t>
-  </si>
-  <si>
-    <t>Långsiktig finansiering av Det finns långsiktig finansiering av föräldraföreläsningar.föräldraföreläsningar </t>
-  </si>
-  <si>
-    <t>Det finns det en struktur för arbetet (Exempelvis samordnare, kompetensutveckling).</t>
-  </si>
-  <si>
     <t>Det görs uppföljning av vilka som tar del av föräldraföreläsningarna.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kommunen erbjuder familjerådgivning.</t>
   </si>
   <si>
     <r>
@@ -312,28 +243,13 @@
     </r>
   </si>
   <si>
-    <t>Det finns det mål/strategier för arbetet med familjerådgivning.</t>
-  </si>
-  <si>
     <t>Barn ges möjlighet att komma till tals i samband familjerådgivning.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifika modeller, metoder, verktyg eller bedömningsinstrument används under samtalen. </t>
-  </si>
-  <si>
     <t>Det görs uppföljning av vilka som deltar i familjerådgivning.</t>
   </si>
   <si>
     <t>Det görs uppföljning av vilket resultat familjerådgivningen får för barn och föräldrar.</t>
-  </si>
-  <si>
-    <t>Samtalsledarna ges möjlighet till kompetensutveckling och vidareutbildning.sledarna</t>
-  </si>
-  <si>
-    <t>Det finns struktur för arbetet (exempelvis återkommande utbildning av gruppledare, samordnare, kompetensutveckling). (FLYTTA TILL FÖRDJUPNING)</t>
-  </si>
-  <si>
-    <t>Kommunen erbjudersamarbetssamtal.</t>
   </si>
   <si>
     <r>
@@ -359,15 +275,9 @@
     </r>
   </si>
   <si>
-    <t>Mål/strategier för arbetet med Det finn mål/strategier för arbetet med samarbetssamtal. samarbetssamtal.</t>
-  </si>
-  <si>
     <t>Barn ges möjlighet att komma till tals i samband samarbetssamtalen.</t>
   </si>
   <si>
-    <t>Samtalsledarna ges möjlighet till kompetensutveckling och vidareutbildning. FÖRDJUPNING</t>
-  </si>
-  <si>
     <t>Det görs uppföljning av vilka som deltar i samarbetssamtal.</t>
   </si>
   <si>
@@ -375,15 +285,6 @@
   </si>
   <si>
     <t>Utökat hembesöksprogram erbjuds i vår kommun.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Öppen förskola </t>
-  </si>
-  <si>
-    <t>Det finns en eller flera öppna förskolor i kommunen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Det finns mål/strategier för arbetet med öppen förskola.</t>
   </si>
   <si>
     <r>
@@ -407,6 +308,167 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>Samordnade insatser runt barn och unga</t>
+  </si>
+  <si>
+    <t>Det finns en överenskommelse rörande samordnade insatser runt barn och ungdomar mellan relevanta aktörer där föräldraskapsstöd ingår.</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med samordnade insatser runt barn och ungdomar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Det finns långsiktig finansiering för samordnade insatser runt barn och ungdomar. </t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av vilka målgrupper som nås genom de samordnade insatserna.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av arbetets resultat för föräldrar, barn och ungdomar.</t>
+  </si>
+  <si>
+    <t>Barn, ungdomar och föräldrar involveras i utformningen av insatserna.</t>
+  </si>
+  <si>
+    <t>Det finns plattformar eller forum för tvärsektoriellt arbete där föräldraskapsstöd ingår.</t>
+  </si>
+  <si>
+    <t>Det finns en samordnare för föräldraskapsstöd.</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med utökat hembesöksprogram.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning  av vilka som besöker familjecentralen.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av familjecentralens resultat för barn och föräldrar</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med familjecentraler.</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med öppen förskola.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Besökare inkluderas i utformning av innehållet i verksamheten. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Det görs kontinuerlig uppföljning av hur vårdnadshavare uppfattar samverkan med förskola/skola. </t>
+  </si>
+  <si>
+    <t>Det finns samverkan mellan kommun och region gällande föräldragrupperna.</t>
+  </si>
+  <si>
+    <t>Det finns mål ochstrategier för arbetet med föräldragrupper.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av vilka resultat som grupperna får för barn och föräldrar.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av vilka som deltar i föräldragrupper på MHV respektive BHV.</t>
+  </si>
+  <si>
+    <t>Barn och föräldrar involveras i utformningen av grupperna.</t>
+  </si>
+  <si>
+    <t>Lilla ABC</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med universella föräldraskapsstödsprogram.</t>
+  </si>
+  <si>
+    <t>Vårdnadshavare och föräldrar involveras i föräldraskapsstödets utformning.</t>
+  </si>
+  <si>
+    <t>Det finns långsiktig finansiering av föräldraföreläsningar</t>
+  </si>
+  <si>
+    <t>Vårdnadshavare samt barn och unga involveras i föräldraföreläsningarnas innehåll och utformning.</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med familjerådgivning.</t>
+  </si>
+  <si>
+    <t>Kommunen erbjuder familjerådgivning.</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med föräldraföreläsningar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standardiserade modeller, metoder, verktyg eller bedömningsinstrument används under samtalen. </t>
+  </si>
+  <si>
+    <t>Kommunen erbjuder samarbetssamtal.</t>
+  </si>
+  <si>
+    <t>Standardiserade modeller, metoder, verktyg eller bedömningsinstrument används under samtalen.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF242424"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Skolsociala team</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF242424"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Det finns skolsociala team i kommunen.</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med skolsociala team</t>
+  </si>
+  <si>
+    <t>Det finns mål och strategier för arbetet med samarbetssamtal.</t>
+  </si>
+  <si>
+    <t>Det finns en långsiktig finansiering för arbetet med skolsociala team.</t>
+  </si>
+  <si>
+    <t>Barn och föräldrar inkluderas i utformningen av de skolsociala teamen.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av vilka målgrupper som får insatser via skolsociala team.</t>
+  </si>
+  <si>
+    <t>Det görs uppföljning av vilket resultat skolsociala team får för barn och föräldrar.</t>
+  </si>
+  <si>
+    <t>Socialt fältarbete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunen arbetar med socialt fältarbete. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Det finns en överenskommelse och rutiner för samverkan mellan fältverksamheten och närliggande verksamhet som exempelvis socialtjänstens myndighetsutövning, öppenvård, skola, polis och fritidsverksamheter centralt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Det finns tydliga rutiner, riktlinjer och mål kring vad det sociala fältarbetet bör innehålla och leda till. </t>
+  </si>
+  <si>
+    <t>Det finns en långsiktig finansiering av fältverksamheten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbetet dokumenteras och följs upp.  </t>
+  </si>
+  <si>
+    <t>Barn och unga involveras i planeringen och genomförandet av organiserade aktiviteter.</t>
   </si>
 </sst>
 </file>
@@ -460,18 +522,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -611,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -661,23 +717,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -690,7 +739,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
@@ -703,10 +751,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1098,11 +1146,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CC34EE-B55D-6C4C-A07E-2F5F91D32621}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -1126,7 +1172,7 @@
       <c r="A4" s="17"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="17">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1141,26 +1187,26 @@
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="61" customHeight="1">
-      <c r="A6" s="25" t="s">
-        <v>18</v>
+      <c r="A6" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" ht="40">
+    <row r="7" spans="1:7" s="14" customFormat="1" ht="80">
       <c r="A7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="60">
+        <v>65</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A8" s="20" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1169,16 +1215,16 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A9" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="20">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A10" s="20" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1187,69 +1233,63 @@
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A11" s="20" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="80">
-      <c r="A12" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" ht="51" customHeight="1">
-      <c r="A13" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="40">
-      <c r="A14" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" s="14" customFormat="1" ht="40">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A12" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A13" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="60">
+      <c r="A14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="20">
       <c r="A15" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" s="14" customFormat="1" ht="40">
-      <c r="A16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" s="8" customFormat="1" ht="51" customHeight="1">
+      <c r="A16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" ht="40">
       <c r="A17" s="19" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1258,108 +1298,108 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A18" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" s="21" customFormat="1" ht="46" customHeight="1">
-      <c r="A19" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
+    <row r="18" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A18" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" s="14" customFormat="1" ht="40">
       <c r="A20" s="19" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="30"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="60">
-      <c r="A21" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A21" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A23" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+    <row r="22" spans="1:7" ht="46" customHeight="1">
+      <c r="A22" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A23" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A24" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="52" customHeight="1">
-      <c r="A25" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" s="14" customFormat="1" ht="40">
-      <c r="A26" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+    <row r="25" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A25" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A26" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A27" s="20" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1368,53 +1408,53 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A28" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A29" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="63" customHeight="1">
-      <c r="A30" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" s="14" customFormat="1" ht="46" customHeight="1">
-      <c r="A31" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="60">
-      <c r="A32" s="20" t="s">
-        <v>43</v>
+    <row r="28" spans="1:7" ht="52" customHeight="1">
+      <c r="A28" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A29" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A30" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A31" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A32" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1423,9 +1463,9 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="80">
-      <c r="A33" s="20" t="s">
-        <v>44</v>
+    <row r="33" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A33" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1434,31 +1474,31 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" ht="80">
-      <c r="A34" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="60">
-      <c r="A35" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="60">
-      <c r="A36" s="28" t="s">
-        <v>47</v>
+    <row r="34" spans="1:7" ht="63" customHeight="1">
+      <c r="A34" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" s="14" customFormat="1" ht="46" customHeight="1">
+      <c r="A35" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="80">
+      <c r="A36" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1467,134 +1507,142 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" s="8" customFormat="1" ht="50" customHeight="1">
-      <c r="A37" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" s="14" customFormat="1" ht="40">
-      <c r="A38" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-    </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A39" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A40" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="40">
-      <c r="A41" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+    <row r="37" spans="1:7" s="5" customFormat="1" ht="60">
+      <c r="A37" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" s="5" customFormat="1" ht="60">
+      <c r="A38" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" s="8" customFormat="1" ht="50" customHeight="1">
+      <c r="A39" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A40" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" s="14" customFormat="1" ht="40">
+      <c r="A41" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A42" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:7" s="8" customFormat="1" ht="61" customHeight="1">
-      <c r="A43" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-    </row>
-    <row r="44" spans="1:7" s="14" customFormat="1" ht="40">
+        <v>81</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" s="5" customFormat="1" ht="40">
+      <c r="A43" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A44" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-    </row>
-    <row r="45" spans="1:7" s="5" customFormat="1" ht="19">
+        <v>83</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A45" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:7" s="5" customFormat="1" ht="19">
+        <v>82</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" s="5" customFormat="1" ht="40">
       <c r="A46" s="20" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" ht="19">
-      <c r="A47" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" ht="19">
-      <c r="A48" s="18"/>
+    <row r="47" spans="1:7" ht="19">
+      <c r="A47" s="18"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" ht="44">
+      <c r="A48" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="44">
-      <c r="A49" s="34" t="s">
-        <v>56</v>
+    <row r="49" spans="1:5" ht="60">
+      <c r="A49" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" ht="60">
-      <c r="A50" s="19" t="s">
-        <v>57</v>
+    <row r="50" spans="1:5" ht="20">
+      <c r="A50" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1602,7 +1650,7 @@
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A51" s="33" t="s">
+      <c r="A51" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="9"/>
@@ -1611,7 +1659,7 @@
       <c r="E51" s="9"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B52" s="9"/>
@@ -1620,7 +1668,7 @@
       <c r="E52" s="9"/>
     </row>
     <row r="53" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B53" s="9"/>
@@ -1629,7 +1677,7 @@
       <c r="E53" s="9"/>
     </row>
     <row r="54" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B54" s="9"/>
@@ -1638,7 +1686,7 @@
       <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="9"/>
@@ -1647,7 +1695,7 @@
       <c r="E55" s="9"/>
     </row>
     <row r="56" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="9"/>
@@ -1656,16 +1704,16 @@
       <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A57" s="33" t="s">
-        <v>54</v>
+      <c r="A57" s="29" t="s">
+        <v>36</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="1:5" s="21" customFormat="1" ht="20">
-      <c r="A58" s="33" t="s">
+    <row r="58" spans="1:5" ht="20">
+      <c r="A58" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B58" s="1"/>
@@ -1675,7 +1723,7 @@
     </row>
     <row r="59" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A59" s="20" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -1684,16 +1732,16 @@
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A60" s="20" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="1:5" s="5" customFormat="1" ht="19">
-      <c r="A61" s="22" t="s">
-        <v>59</v>
+    <row r="61" spans="1:5" s="5" customFormat="1" ht="60">
+      <c r="A61" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -1702,7 +1750,7 @@
     </row>
     <row r="62" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A62" s="20" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -1711,43 +1759,43 @@
     </row>
     <row r="63" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A63" s="20" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="1:5" s="36" customFormat="1" ht="53" customHeight="1">
-      <c r="A64" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-    </row>
-    <row r="65" spans="1:5" ht="39" customHeight="1">
-      <c r="A65" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A66" s="33" t="s">
+    <row r="64" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A64" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+    </row>
+    <row r="65" spans="1:5" s="32" customFormat="1" ht="53" customHeight="1">
+      <c r="A65" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+    </row>
+    <row r="66" spans="1:5" ht="39" customHeight="1">
+      <c r="A66" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" s="5" customFormat="1" ht="20">
+      <c r="A67" s="29" t="s">
         <v>13</v>
-      </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-    </row>
-    <row r="67" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A67" s="33" t="s">
-        <v>14</v>
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -1755,8 +1803,8 @@
       <c r="E67" s="9"/>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A68" s="33" t="s">
-        <v>64</v>
+      <c r="A68" s="29" t="s">
+        <v>14</v>
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -1764,8 +1812,8 @@
       <c r="E68" s="9"/>
     </row>
     <row r="69" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A69" s="33" t="s">
-        <v>63</v>
+      <c r="A69" s="29" t="s">
+        <v>45</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -1773,8 +1821,8 @@
       <c r="E69" s="9"/>
     </row>
     <row r="70" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A70" s="33" t="s">
-        <v>15</v>
+      <c r="A70" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -1782,8 +1830,8 @@
       <c r="E70" s="9"/>
     </row>
     <row r="71" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A71" s="33" t="s">
-        <v>65</v>
+      <c r="A71" s="29" t="s">
+        <v>15</v>
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -1791,17 +1839,17 @@
       <c r="E71" s="9"/>
     </row>
     <row r="72" spans="1:5" s="5" customFormat="1" ht="20">
-      <c r="A72" s="33" t="s">
-        <v>16</v>
+      <c r="A72" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="1:5" s="5" customFormat="1" ht="40">
-      <c r="A73" s="20" t="s">
-        <v>66</v>
+    <row r="73" spans="1:5" s="5" customFormat="1" ht="20">
+      <c r="A73" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -1810,16 +1858,16 @@
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A74" s="20" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:5" s="5" customFormat="1" ht="19">
-      <c r="A75" s="22" t="s">
-        <v>84</v>
+    <row r="75" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A75" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -1828,130 +1876,130 @@
     </row>
     <row r="76" spans="1:5" s="5" customFormat="1" ht="38" customHeight="1">
       <c r="A76" s="20" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="1:5" s="5" customFormat="1" ht="40">
+    <row r="77" spans="1:5" s="5" customFormat="1" ht="38" customHeight="1">
       <c r="A77" s="20" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:5" s="37" customFormat="1" ht="61" customHeight="1">
-      <c r="A78" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-    </row>
-    <row r="79" spans="1:5" s="14" customFormat="1" ht="40">
-      <c r="A79" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="23"/>
-    </row>
-    <row r="80" spans="1:5" s="5" customFormat="1" ht="40">
-      <c r="A80" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-    </row>
-    <row r="81" spans="1:5" s="5" customFormat="1" ht="60">
+    <row r="78" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A78" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="1:5" s="32" customFormat="1" ht="61" customHeight="1">
+      <c r="A79" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+    </row>
+    <row r="80" spans="1:5" s="14" customFormat="1" ht="40">
+      <c r="A80" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+    </row>
+    <row r="81" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A81" s="20" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="1:5" s="5" customFormat="1" ht="49" customHeight="1">
-      <c r="A82" s="22" t="s">
-        <v>74</v>
+    <row r="82" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A82" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="1:5" s="5" customFormat="1" ht="40">
+    <row r="83" spans="1:5" s="5" customFormat="1" ht="49" customHeight="1">
       <c r="A83" s="20" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="1:5">
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:5" s="21" customFormat="1" ht="44">
-      <c r="A85" s="38" t="s">
-        <v>77</v>
-      </c>
+    <row r="84" spans="1:5" s="5" customFormat="1" ht="60">
+      <c r="A84" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+    </row>
+    <row r="85" spans="1:5">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5" s="14" customFormat="1" ht="19">
-      <c r="A86" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B86" s="23"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
-      <c r="E86" s="23"/>
-    </row>
-    <row r="87" spans="1:5" s="5" customFormat="1" ht="40">
-      <c r="A87" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
+    <row r="86" spans="1:5" ht="44">
+      <c r="A86" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" s="14" customFormat="1" ht="20">
+      <c r="A87" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
     </row>
     <row r="88" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A88" s="20" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="1:5" s="5" customFormat="1" ht="60">
+    <row r="89" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A89" s="20" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="1:5" s="5" customFormat="1" ht="40">
+    <row r="90" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A90" s="20" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -1960,16 +2008,16 @@
     </row>
     <row r="91" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A91" s="20" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="1:5" s="5" customFormat="1" ht="60">
-      <c r="A92" s="22" t="s">
-        <v>83</v>
+    <row r="92" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A92" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -1982,9 +2030,9 @@
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="1:5" s="21" customFormat="1" ht="44">
-      <c r="A94" s="38" t="s">
-        <v>86</v>
+    <row r="94" spans="1:5" ht="44">
+      <c r="A94" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1993,16 +2041,16 @@
     </row>
     <row r="95" spans="1:5" s="14" customFormat="1" ht="20">
       <c r="A95" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B95" s="23"/>
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23"/>
-    </row>
-    <row r="96" spans="1:5" s="5" customFormat="1" ht="60">
+        <v>94</v>
+      </c>
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+    </row>
+    <row r="96" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A96" s="20" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -2011,7 +2059,7 @@
     </row>
     <row r="97" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A97" s="20" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -2020,7 +2068,7 @@
     </row>
     <row r="98" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A98" s="20" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -2029,30 +2077,159 @@
     </row>
     <row r="99" spans="1:5" s="5" customFormat="1" ht="40">
       <c r="A99" s="20" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="1:5" s="5" customFormat="1" ht="19">
-      <c r="A100" s="22" t="s">
-        <v>89</v>
+    <row r="100" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A100" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
     </row>
-    <row r="101" spans="1:5" s="5" customFormat="1" ht="40">
-      <c r="A101" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
+    <row r="101" spans="1:5">
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" ht="44">
+      <c r="A102" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" s="14" customFormat="1" ht="19">
+      <c r="A103" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+    </row>
+    <row r="104" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A104" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+    </row>
+    <row r="105" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A105" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="9"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+    </row>
+    <row r="106" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A106" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106" s="9"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+    </row>
+    <row r="107" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A107" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+    </row>
+    <row r="108" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A108" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" ht="22">
+      <c r="A110" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" s="14" customFormat="1" ht="19">
+      <c r="A111" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
+      <c r="E111" s="21"/>
+    </row>
+    <row r="112" spans="1:5" s="5" customFormat="1" ht="98" customHeight="1">
+      <c r="A112" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+    </row>
+    <row r="113" spans="1:5" s="5" customFormat="1" ht="60">
+      <c r="A113" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="9"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+    </row>
+    <row r="114" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A114" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B114" s="9"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+    </row>
+    <row r="115" spans="1:5" s="5" customFormat="1" ht="20">
+      <c r="A115" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B115" s="9"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+    </row>
+    <row r="116" spans="1:5" s="5" customFormat="1" ht="40">
+      <c r="A116" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B116" s="9"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>